<commit_message>
modifique los titulos del excel
</commit_message>
<xml_diff>
--- a/excel/resultado_consulta.xlsx
+++ b/excel/resultado_consulta.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>#</t>
   </si>
@@ -22,31 +22,37 @@
     <t>Cod restaurante</t>
   </si>
   <si>
-    <t>Lectura actual</t>
-  </si>
-  <si>
-    <t>Lectura anterior</t>
-  </si>
-  <si>
-    <t>Consumo</t>
-  </si>
-  <si>
-    <t>Vertimiento</t>
-  </si>
-  <si>
-    <t>Total a pagar</t>
-  </si>
-  <si>
-    <t>fecha</t>
+    <t>Lectura Inicial</t>
+  </si>
+  <si>
+    <t>Lectura Final</t>
+  </si>
+  <si>
+    <t>Causa mes</t>
+  </si>
+  <si>
+    <t>Consumo mes</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>Alumbrado</t>
+  </si>
+  <si>
+    <t>Kw/h</t>
+  </si>
+  <si>
+    <t>Valor de Kw/h</t>
+  </si>
+  <si>
+    <t>Direccion</t>
   </si>
   <si>
     <t>2020-08-29</t>
   </si>
   <si>
     <t>2020-09-28</t>
-  </si>
-  <si>
-    <t>CRA 13 # 22 B- 11 LC 1- LC 2 LC 00 AV 30 AG</t>
   </si>
   <si>
     <t>CRA 13 # 22 B- 11 LC 1-LC 2 LC 00 AV 30 AG</t>
@@ -381,13 +387,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,19 +418,28 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>6513075</v>
@@ -441,22 +456,19 @@
       <c r="I2">
         <v>8680</v>
       </c>
-      <c r="J2" t="s">
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>6513075</v>
@@ -473,22 +485,19 @@
       <c r="I3">
         <v>8680</v>
       </c>
-      <c r="J3" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:11">
       <c r="A4">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E4">
         <v>6513075</v>
@@ -505,22 +514,22 @@
       <c r="I4">
         <v>8680</v>
       </c>
-      <c r="J4" t="s">
-        <v>10</v>
+      <c r="J4">
+        <v>602.9728</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:11">
       <c r="A5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E5">
         <v>6513075</v>
@@ -537,22 +546,22 @@
       <c r="I5">
         <v>8680</v>
       </c>
-      <c r="J5" t="s">
-        <v>10</v>
+      <c r="J5">
+        <v>602.9728</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:11">
       <c r="A6">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E6">
         <v>6513075</v>
@@ -569,22 +578,22 @@
       <c r="I6">
         <v>8680</v>
       </c>
-      <c r="J6" t="s">
-        <v>10</v>
+      <c r="J6">
+        <v>602.9728</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:11">
       <c r="A7">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>6513075</v>
@@ -601,72 +610,11 @@
       <c r="I7">
         <v>8680</v>
       </c>
-      <c r="J7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8">
-        <v>6513075</v>
-      </c>
-      <c r="F8">
-        <v>5233804</v>
-      </c>
-      <c r="G8">
-        <v>1046761</v>
-      </c>
-      <c r="H8">
-        <v>197790</v>
-      </c>
-      <c r="I8">
-        <v>8680</v>
-      </c>
-      <c r="J8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9">
-        <v>6513075</v>
-      </c>
-      <c r="F9">
-        <v>5233804</v>
-      </c>
-      <c r="G9">
-        <v>1046761</v>
-      </c>
-      <c r="H9">
-        <v>197790</v>
-      </c>
-      <c r="I9">
-        <v>8680</v>
-      </c>
-      <c r="J9" t="s">
-        <v>11</v>
+      <c r="J7">
+        <v>602.9728</v>
+      </c>
+      <c r="K7" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
consultar por nombre de meses no por numero
</commit_message>
<xml_diff>
--- a/excel/resultado_consulta.xlsx
+++ b/excel/resultado_consulta.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>#</t>
   </si>
@@ -47,15 +47,6 @@
   </si>
   <si>
     <t>Direccion</t>
-  </si>
-  <si>
-    <t>2020-08-29</t>
-  </si>
-  <si>
-    <t>2020-09-28</t>
-  </si>
-  <si>
-    <t>CRA 13 # 22 B- 11 LC 1-LC 2 LC 00 AV 30 AG</t>
   </si>
 </sst>
 </file>
@@ -387,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -428,195 +419,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>6513075</v>
-      </c>
-      <c r="F2">
-        <v>5233804</v>
-      </c>
-      <c r="G2">
-        <v>1046761</v>
-      </c>
-      <c r="H2">
-        <v>197790</v>
-      </c>
-      <c r="I2">
-        <v>8680</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>6513075</v>
-      </c>
-      <c r="F3">
-        <v>5233804</v>
-      </c>
-      <c r="G3">
-        <v>1046761</v>
-      </c>
-      <c r="H3">
-        <v>197790</v>
-      </c>
-      <c r="I3">
-        <v>8680</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>6513075</v>
-      </c>
-      <c r="F4">
-        <v>5233804</v>
-      </c>
-      <c r="G4">
-        <v>1046761</v>
-      </c>
-      <c r="H4">
-        <v>197790</v>
-      </c>
-      <c r="I4">
-        <v>8680</v>
-      </c>
-      <c r="J4">
-        <v>602.9728</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
-      <c r="A5">
-        <v>12</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>6513075</v>
-      </c>
-      <c r="F5">
-        <v>5233804</v>
-      </c>
-      <c r="G5">
-        <v>1046761</v>
-      </c>
-      <c r="H5">
-        <v>197790</v>
-      </c>
-      <c r="I5">
-        <v>8680</v>
-      </c>
-      <c r="J5">
-        <v>602.9728</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6">
-        <v>13</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>6513075</v>
-      </c>
-      <c r="F6">
-        <v>5233804</v>
-      </c>
-      <c r="G6">
-        <v>1046761</v>
-      </c>
-      <c r="H6">
-        <v>197790</v>
-      </c>
-      <c r="I6">
-        <v>8680</v>
-      </c>
-      <c r="J6">
-        <v>602.9728</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>6513075</v>
-      </c>
-      <c r="F7">
-        <v>5233804</v>
-      </c>
-      <c r="G7">
-        <v>1046761</v>
-      </c>
-      <c r="H7">
-        <v>197790</v>
-      </c>
-      <c r="I7">
-        <v>8680</v>
-      </c>
-      <c r="J7">
-        <v>602.9728</v>
-      </c>
-      <c r="K7" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>